<commit_message>
Updated team retention data
</commit_message>
<xml_diff>
--- a/Docs/Data/Team Retention.xlsx
+++ b/Docs/Data/Team Retention.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vws1\Documents\Personal\Soccer\GKSSA-Stats-Calculator\Docs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9960274A-B96D-459A-92BC-6EB1678671FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537B059B-7E6C-4944-9944-62D822C7D55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{7844BBDF-6516-4F3E-ACF8-72B0D7E6BADF}"/>
   </bookViews>
@@ -1135,11 +1135,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1147,14 +1153,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4028,7 +4028,7 @@
   <dimension ref="A1:J357"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F163" sqref="F163"/>
     </sheetView>
   </sheetViews>
@@ -4050,11 +4050,11 @@
       <c r="C1" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="I1" s="24" t="s">
         <v>113</v>
       </c>
@@ -4064,7 +4064,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="45" t="s">
         <v>72</v>
       </c>
       <c r="B2" s="2">
@@ -4093,7 +4093,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="45" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="2">
@@ -4116,7 +4116,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="45" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2">
@@ -4139,7 +4139,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="45" t="s">
         <v>104</v>
       </c>
       <c r="B5" s="2">
@@ -4162,7 +4162,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="45" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="2">
@@ -4185,7 +4185,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="45" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="2">
@@ -4208,7 +4208,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="45" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="2">
@@ -4231,7 +4231,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="45" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="2">
@@ -4254,7 +4254,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="45" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="2">
@@ -4277,7 +4277,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="45" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="2">
@@ -4300,7 +4300,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="45" t="s">
         <v>63</v>
       </c>
       <c r="B12" s="2">
@@ -4323,7 +4323,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="45" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2">
@@ -4346,7 +4346,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="45" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="2">
@@ -4369,7 +4369,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="45" t="s">
         <v>93</v>
       </c>
       <c r="B15" s="2">
@@ -4392,7 +4392,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="45" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="2">
@@ -4415,7 +4415,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="45" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="2">
@@ -4438,7 +4438,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="45" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="2">
@@ -4461,7 +4461,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="45" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="2">
@@ -4484,7 +4484,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="45" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="2">
@@ -4507,7 +4507,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="45" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="2">
@@ -4530,7 +4530,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="45" t="s">
         <v>205</v>
       </c>
       <c r="B22" s="2">
@@ -4553,7 +4553,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="45" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2">
@@ -4576,7 +4576,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="45" t="s">
         <v>103</v>
       </c>
       <c r="B24" s="2">
@@ -4589,7 +4589,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="45" t="s">
         <v>53</v>
       </c>
       <c r="B25" s="2">
@@ -4602,7 +4602,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="45" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="2">
@@ -4615,7 +4615,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="45" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="2">
@@ -4628,7 +4628,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="45" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="2">
@@ -4641,7 +4641,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="45" t="s">
         <v>57</v>
       </c>
       <c r="B29" s="2">
@@ -4654,7 +4654,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="45" t="s">
         <v>165</v>
       </c>
       <c r="B30" s="2">
@@ -4667,7 +4667,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="45" t="s">
         <v>186</v>
       </c>
       <c r="B31" s="2">
@@ -4680,7 +4680,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="45" t="s">
         <v>163</v>
       </c>
       <c r="B32" s="2">
@@ -4693,7 +4693,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="45" t="s">
         <v>69</v>
       </c>
       <c r="B33" s="2">
@@ -4706,7 +4706,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="45" t="s">
         <v>164</v>
       </c>
       <c r="B34" s="2">
@@ -4719,7 +4719,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="2">
@@ -4732,7 +4732,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="45" t="s">
         <v>75</v>
       </c>
       <c r="B36" s="2">
@@ -4745,7 +4745,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="45" t="s">
         <v>27</v>
       </c>
       <c r="B37" s="2">
@@ -4758,7 +4758,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="45" t="s">
         <v>59</v>
       </c>
       <c r="B38" s="2">
@@ -4771,7 +4771,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="45" t="s">
         <v>148</v>
       </c>
       <c r="B39" s="2">
@@ -4784,7 +4784,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="45" t="s">
         <v>129</v>
       </c>
       <c r="B40" s="2">
@@ -4797,7 +4797,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="51" t="s">
+      <c r="A41" s="45" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="2">
@@ -4810,7 +4810,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="45" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="2">
@@ -4823,7 +4823,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="51" t="s">
+      <c r="A43" s="45" t="s">
         <v>136</v>
       </c>
       <c r="B43" s="2">
@@ -4836,7 +4836,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="45" t="s">
         <v>68</v>
       </c>
       <c r="B44" s="2">
@@ -4849,7 +4849,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="45" t="s">
         <v>31</v>
       </c>
       <c r="B45" s="2">
@@ -4862,7 +4862,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="45" t="s">
         <v>204</v>
       </c>
       <c r="B46" s="2">
@@ -4875,7 +4875,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="51" t="s">
+      <c r="A47" s="45" t="s">
         <v>82</v>
       </c>
       <c r="B47" s="2">
@@ -4888,7 +4888,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="51" t="s">
+      <c r="A48" s="45" t="s">
         <v>10</v>
       </c>
       <c r="B48" s="2">
@@ -4901,7 +4901,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="51" t="s">
+      <c r="A49" s="45" t="s">
         <v>101</v>
       </c>
       <c r="B49" s="2">
@@ -4914,7 +4914,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="51" t="s">
+      <c r="A50" s="45" t="s">
         <v>89</v>
       </c>
       <c r="B50" s="2">
@@ -4927,7 +4927,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="51" t="s">
+      <c r="A51" s="45" t="s">
         <v>37</v>
       </c>
       <c r="B51" s="2">
@@ -4940,7 +4940,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="45" t="s">
         <v>96</v>
       </c>
       <c r="B52" s="2">
@@ -4953,7 +4953,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="51" t="s">
+      <c r="A53" s="45" t="s">
         <v>139</v>
       </c>
       <c r="B53" s="2">
@@ -4966,7 +4966,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="51" t="s">
+      <c r="A54" s="45" t="s">
         <v>151</v>
       </c>
       <c r="B54" s="2">
@@ -4979,7 +4979,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="51" t="s">
+      <c r="A55" s="45" t="s">
         <v>92</v>
       </c>
       <c r="B55" s="2">
@@ -4992,7 +4992,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="51" t="s">
+      <c r="A56" s="45" t="s">
         <v>25</v>
       </c>
       <c r="B56" s="2">
@@ -5005,7 +5005,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="51" t="s">
+      <c r="A57" s="45" t="s">
         <v>195</v>
       </c>
       <c r="B57" s="2">
@@ -5018,7 +5018,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="51" t="s">
+      <c r="A58" s="45" t="s">
         <v>200</v>
       </c>
       <c r="B58" s="2">
@@ -5031,7 +5031,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="51" t="s">
+      <c r="A59" s="45" t="s">
         <v>138</v>
       </c>
       <c r="B59" s="2">
@@ -5044,7 +5044,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="51" t="s">
+      <c r="A60" s="45" t="s">
         <v>189</v>
       </c>
       <c r="B60" s="2">
@@ -5057,7 +5057,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="51" t="s">
+      <c r="A61" s="45" t="s">
         <v>88</v>
       </c>
       <c r="B61" s="2">
@@ -5070,7 +5070,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="51" t="s">
+      <c r="A62" s="45" t="s">
         <v>21</v>
       </c>
       <c r="B62" s="2">
@@ -5083,7 +5083,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="51" t="s">
+      <c r="A63" s="45" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="2">
@@ -5096,7 +5096,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="51" t="s">
+      <c r="A64" s="45" t="s">
         <v>133</v>
       </c>
       <c r="B64" s="2">
@@ -5109,7 +5109,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="51" t="s">
+      <c r="A65" s="45" t="s">
         <v>190</v>
       </c>
       <c r="B65" s="2">
@@ -5122,7 +5122,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="51" t="s">
+      <c r="A66" s="45" t="s">
         <v>167</v>
       </c>
       <c r="B66" s="2">
@@ -5135,7 +5135,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="51" t="s">
+      <c r="A67" s="45" t="s">
         <v>176</v>
       </c>
       <c r="B67" s="2">
@@ -5148,7 +5148,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="51" t="s">
+      <c r="A68" s="45" t="s">
         <v>156</v>
       </c>
       <c r="B68" s="2">
@@ -5161,7 +5161,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="51" t="s">
+      <c r="A69" s="45" t="s">
         <v>171</v>
       </c>
       <c r="B69" s="2">
@@ -5174,7 +5174,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="51" t="s">
+      <c r="A70" s="45" t="s">
         <v>22</v>
       </c>
       <c r="B70" s="2">
@@ -5187,7 +5187,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="51" t="s">
+      <c r="A71" s="45" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="2">
@@ -5200,7 +5200,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="51" t="s">
+      <c r="A72" s="45" t="s">
         <v>41</v>
       </c>
       <c r="B72" s="2">
@@ -5213,7 +5213,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="51" t="s">
+      <c r="A73" s="45" t="s">
         <v>87</v>
       </c>
       <c r="B73" s="2">
@@ -5226,7 +5226,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="51" t="s">
+      <c r="A74" s="45" t="s">
         <v>158</v>
       </c>
       <c r="B74" s="2">
@@ -5239,7 +5239,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="51" t="s">
+      <c r="A75" s="45" t="s">
         <v>60</v>
       </c>
       <c r="B75" s="2">
@@ -5252,7 +5252,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="51" t="s">
+      <c r="A76" s="45" t="s">
         <v>71</v>
       </c>
       <c r="B76" s="2">
@@ -5265,7 +5265,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="51" t="s">
+      <c r="A77" s="45" t="s">
         <v>95</v>
       </c>
       <c r="B77" s="2">
@@ -5278,7 +5278,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="51" t="s">
+      <c r="A78" s="45" t="s">
         <v>85</v>
       </c>
       <c r="B78" s="2">
@@ -5291,7 +5291,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="51" t="s">
+      <c r="A79" s="45" t="s">
         <v>32</v>
       </c>
       <c r="B79" s="2">
@@ -5304,7 +5304,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="51" t="s">
+      <c r="A80" s="45" t="s">
         <v>86</v>
       </c>
       <c r="B80" s="2">
@@ -5317,7 +5317,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="51" t="s">
+      <c r="A81" s="45" t="s">
         <v>102</v>
       </c>
       <c r="B81" s="2">
@@ -5330,7 +5330,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="51" t="s">
+      <c r="A82" s="45" t="s">
         <v>16</v>
       </c>
       <c r="B82" s="2">
@@ -5343,7 +5343,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="51" t="s">
+      <c r="A83" s="45" t="s">
         <v>35</v>
       </c>
       <c r="B83" s="2">
@@ -5356,7 +5356,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="51" t="s">
+      <c r="A84" s="45" t="s">
         <v>184</v>
       </c>
       <c r="B84" s="2">
@@ -5369,7 +5369,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="51" t="s">
+      <c r="A85" s="45" t="s">
         <v>5</v>
       </c>
       <c r="B85" s="2">
@@ -5382,7 +5382,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="51" t="s">
+      <c r="A86" s="45" t="s">
         <v>36</v>
       </c>
       <c r="B86" s="2">
@@ -5395,7 +5395,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="51" t="s">
+      <c r="A87" s="45" t="s">
         <v>51</v>
       </c>
       <c r="B87" s="2">
@@ -5408,7 +5408,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="51" t="s">
+      <c r="A88" s="45" t="s">
         <v>30</v>
       </c>
       <c r="B88" s="2">
@@ -5421,7 +5421,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="51" t="s">
+      <c r="A89" s="45" t="s">
         <v>183</v>
       </c>
       <c r="B89" s="2">
@@ -5434,7 +5434,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="51" t="s">
+      <c r="A90" s="45" t="s">
         <v>90</v>
       </c>
       <c r="B90" s="2">
@@ -5447,7 +5447,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="51" t="s">
+      <c r="A91" s="45" t="s">
         <v>173</v>
       </c>
       <c r="B91" s="2">
@@ -5460,7 +5460,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="51" t="s">
+      <c r="A92" s="45" t="s">
         <v>78</v>
       </c>
       <c r="B92" s="2">
@@ -5473,7 +5473,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="51" t="s">
+      <c r="A93" s="45" t="s">
         <v>152</v>
       </c>
       <c r="B93" s="2">
@@ -5486,7 +5486,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="51" t="s">
+      <c r="A94" s="45" t="s">
         <v>20</v>
       </c>
       <c r="B94" s="2">
@@ -5499,7 +5499,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="51" t="s">
+      <c r="A95" s="45" t="s">
         <v>162</v>
       </c>
       <c r="B95" s="2">
@@ -5512,7 +5512,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="51" t="s">
+      <c r="A96" s="45" t="s">
         <v>160</v>
       </c>
       <c r="B96" s="2">
@@ -5525,7 +5525,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="51" t="s">
+      <c r="A97" s="45" t="s">
         <v>198</v>
       </c>
       <c r="B97" s="2">
@@ -5538,7 +5538,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="51" t="s">
+      <c r="A98" s="45" t="s">
         <v>208</v>
       </c>
       <c r="B98" s="2">
@@ -5551,7 +5551,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="51" t="s">
+      <c r="A99" s="45" t="s">
         <v>17</v>
       </c>
       <c r="B99" s="2">
@@ -5564,7 +5564,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="51" t="s">
+      <c r="A100" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B100" s="2">
@@ -5577,7 +5577,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="51" t="s">
+      <c r="A101" s="45" t="s">
         <v>28</v>
       </c>
       <c r="B101" s="2">
@@ -5590,7 +5590,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="51" t="s">
+      <c r="A102" s="45" t="s">
         <v>44</v>
       </c>
       <c r="B102" s="2">
@@ -5603,7 +5603,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="51" t="s">
+      <c r="A103" s="45" t="s">
         <v>48</v>
       </c>
       <c r="B103" s="2">
@@ -5616,7 +5616,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="51" t="s">
+      <c r="A104" s="45" t="s">
         <v>39</v>
       </c>
       <c r="B104" s="2">
@@ -5629,7 +5629,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="51" t="s">
+      <c r="A105" s="45" t="s">
         <v>141</v>
       </c>
       <c r="B105" s="2">
@@ -5642,7 +5642,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="51" t="s">
+      <c r="A106" s="45" t="s">
         <v>45</v>
       </c>
       <c r="B106" s="2">
@@ -5655,7 +5655,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="51" t="s">
+      <c r="A107" s="45" t="s">
         <v>62</v>
       </c>
       <c r="B107" s="2">
@@ -5668,7 +5668,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="51" t="s">
+      <c r="A108" s="45" t="s">
         <v>175</v>
       </c>
       <c r="B108" s="2">
@@ -5681,7 +5681,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="51" t="s">
+      <c r="A109" s="45" t="s">
         <v>181</v>
       </c>
       <c r="B109" s="2">
@@ -5694,7 +5694,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="51" t="s">
+      <c r="A110" s="45" t="s">
         <v>149</v>
       </c>
       <c r="B110" s="2">
@@ -5707,7 +5707,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="51" t="s">
+      <c r="A111" s="45" t="s">
         <v>179</v>
       </c>
       <c r="B111" s="2">
@@ -5720,7 +5720,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="51" t="s">
+      <c r="A112" s="45" t="s">
         <v>170</v>
       </c>
       <c r="B112" s="2">
@@ -5733,7 +5733,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="51" t="s">
+      <c r="A113" s="45" t="s">
         <v>4</v>
       </c>
       <c r="B113" s="2">
@@ -5746,7 +5746,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="51" t="s">
+      <c r="A114" s="45" t="s">
         <v>13</v>
       </c>
       <c r="B114" s="2">
@@ -5759,7 +5759,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="51" t="s">
+      <c r="A115" s="45" t="s">
         <v>73</v>
       </c>
       <c r="B115" s="2">
@@ -5772,7 +5772,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="51" t="s">
+      <c r="A116" s="45" t="s">
         <v>79</v>
       </c>
       <c r="B116" s="2">
@@ -5785,7 +5785,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="51" t="s">
+      <c r="A117" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B117" s="2">
@@ -5798,7 +5798,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" s="51" t="s">
+      <c r="A118" s="45" t="s">
         <v>23</v>
       </c>
       <c r="B118" s="2">
@@ -5811,7 +5811,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="51" t="s">
+      <c r="A119" s="45" t="s">
         <v>143</v>
       </c>
       <c r="B119" s="2">
@@ -5824,7 +5824,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="51" t="s">
+      <c r="A120" s="45" t="s">
         <v>2</v>
       </c>
       <c r="B120" s="2">
@@ -5837,7 +5837,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="51" t="s">
+      <c r="A121" s="45" t="s">
         <v>185</v>
       </c>
       <c r="B121" s="2">
@@ -5850,7 +5850,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A122" s="51" t="s">
+      <c r="A122" s="45" t="s">
         <v>142</v>
       </c>
       <c r="B122" s="2">
@@ -5863,7 +5863,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="51" t="s">
+      <c r="A123" s="45" t="s">
         <v>49</v>
       </c>
       <c r="B123" s="2">
@@ -5876,7 +5876,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="51" t="s">
+      <c r="A124" s="45" t="s">
         <v>65</v>
       </c>
       <c r="B124" s="2">
@@ -5889,7 +5889,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" s="51" t="s">
+      <c r="A125" s="45" t="s">
         <v>182</v>
       </c>
       <c r="B125" s="2">
@@ -5902,7 +5902,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="51" t="s">
+      <c r="A126" s="45" t="s">
         <v>180</v>
       </c>
       <c r="B126" s="2">
@@ -5915,7 +5915,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="51" t="s">
+      <c r="A127" s="45" t="s">
         <v>159</v>
       </c>
       <c r="B127" s="2">
@@ -5928,7 +5928,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A128" s="51" t="s">
+      <c r="A128" s="45" t="s">
         <v>168</v>
       </c>
       <c r="B128" s="2">
@@ -5941,7 +5941,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" s="51" t="s">
+      <c r="A129" s="45" t="s">
         <v>196</v>
       </c>
       <c r="B129" s="2">
@@ -5954,7 +5954,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" s="51" t="s">
+      <c r="A130" s="45" t="s">
         <v>38</v>
       </c>
       <c r="B130" s="2">
@@ -5967,7 +5967,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" s="51" t="s">
+      <c r="A131" s="45" t="s">
         <v>84</v>
       </c>
       <c r="B131" s="2">
@@ -5980,7 +5980,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" s="51" t="s">
+      <c r="A132" s="45" t="s">
         <v>178</v>
       </c>
       <c r="B132" s="2">
@@ -5993,7 +5993,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" s="51" t="s">
+      <c r="A133" s="45" t="s">
         <v>67</v>
       </c>
       <c r="B133" s="2">
@@ -6006,7 +6006,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" s="51" t="s">
+      <c r="A134" s="45" t="s">
         <v>97</v>
       </c>
       <c r="B134" s="2">
@@ -6019,7 +6019,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" s="51" t="s">
+      <c r="A135" s="45" t="s">
         <v>105</v>
       </c>
       <c r="B135" s="2">
@@ -6032,7 +6032,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A136" s="51" t="s">
+      <c r="A136" s="45" t="s">
         <v>155</v>
       </c>
       <c r="B136" s="2">
@@ -6045,7 +6045,7 @@
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" s="51" t="s">
+      <c r="A137" s="45" t="s">
         <v>166</v>
       </c>
       <c r="B137" s="2">
@@ -6058,7 +6058,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A138" s="51" t="s">
+      <c r="A138" s="45" t="s">
         <v>11</v>
       </c>
       <c r="B138" s="2">
@@ -6071,7 +6071,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" s="51" t="s">
+      <c r="A139" s="45" t="s">
         <v>99</v>
       </c>
       <c r="B139" s="2">
@@ -6084,7 +6084,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" s="51" t="s">
+      <c r="A140" s="45" t="s">
         <v>66</v>
       </c>
       <c r="B140" s="2">
@@ -6097,7 +6097,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" s="51" t="s">
+      <c r="A141" s="45" t="s">
         <v>153</v>
       </c>
       <c r="B141" s="2">
@@ -6110,7 +6110,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="51" t="s">
+      <c r="A142" s="45" t="s">
         <v>132</v>
       </c>
       <c r="B142" s="2">
@@ -6123,7 +6123,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" s="51" t="s">
+      <c r="A143" s="45" t="s">
         <v>177</v>
       </c>
       <c r="B143" s="2">
@@ -6136,7 +6136,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" s="51" t="s">
+      <c r="A144" s="45" t="s">
         <v>172</v>
       </c>
       <c r="B144" s="2">
@@ -6149,7 +6149,7 @@
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" s="51" t="s">
+      <c r="A145" s="45" t="s">
         <v>201</v>
       </c>
       <c r="B145" s="2">
@@ -6162,7 +6162,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" s="51" t="s">
+      <c r="A146" s="45" t="s">
         <v>191</v>
       </c>
       <c r="B146" s="2">
@@ -6175,7 +6175,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" s="51" t="s">
+      <c r="A147" s="45" t="s">
         <v>147</v>
       </c>
       <c r="B147" s="2">
@@ -6188,7 +6188,7 @@
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A148" s="51" t="s">
+      <c r="A148" s="45" t="s">
         <v>0</v>
       </c>
       <c r="B148" s="2">
@@ -6201,7 +6201,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" s="51" t="s">
+      <c r="A149" s="45" t="s">
         <v>64</v>
       </c>
       <c r="B149" s="2">
@@ -6214,7 +6214,7 @@
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="51" t="s">
+      <c r="A150" s="45" t="s">
         <v>137</v>
       </c>
       <c r="B150" s="2">
@@ -6227,7 +6227,7 @@
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" s="51" t="s">
+      <c r="A151" s="45" t="s">
         <v>157</v>
       </c>
       <c r="B151" s="2">
@@ -6240,7 +6240,7 @@
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" s="51" t="s">
+      <c r="A152" s="45" t="s">
         <v>145</v>
       </c>
       <c r="B152" s="2">
@@ -6253,7 +6253,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="51" t="s">
+      <c r="A153" s="45" t="s">
         <v>150</v>
       </c>
       <c r="B153" s="2">
@@ -6266,7 +6266,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="51" t="s">
+      <c r="A154" s="45" t="s">
         <v>56</v>
       </c>
       <c r="B154" s="2">
@@ -6279,7 +6279,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A155" s="51" t="s">
+      <c r="A155" s="45" t="s">
         <v>130</v>
       </c>
       <c r="B155" s="2">
@@ -6292,7 +6292,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" s="51" t="s">
+      <c r="A156" s="45" t="s">
         <v>197</v>
       </c>
       <c r="B156" s="2">
@@ -6305,7 +6305,7 @@
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" s="51" t="s">
+      <c r="A157" s="45" t="s">
         <v>29</v>
       </c>
       <c r="B157" s="2">
@@ -6318,7 +6318,7 @@
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A158" s="51" t="s">
+      <c r="A158" s="45" t="s">
         <v>140</v>
       </c>
       <c r="B158" s="2">
@@ -6331,7 +6331,7 @@
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A159" s="51" t="s">
+      <c r="A159" s="45" t="s">
         <v>98</v>
       </c>
       <c r="B159" s="2">
@@ -6344,7 +6344,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A160" s="51" t="s">
+      <c r="A160" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B160" s="2">
@@ -6357,7 +6357,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A161" s="51" t="s">
+      <c r="A161" s="45" t="s">
         <v>74</v>
       </c>
       <c r="B161" s="2">
@@ -6370,7 +6370,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" s="51" t="s">
+      <c r="A162" s="45" t="s">
         <v>187</v>
       </c>
       <c r="B162" s="2">
@@ -6383,7 +6383,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" s="51" t="s">
+      <c r="A163" s="45" t="s">
         <v>18</v>
       </c>
       <c r="B163" s="2">
@@ -6396,7 +6396,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" s="51" t="s">
+      <c r="A164" s="45" t="s">
         <v>81</v>
       </c>
       <c r="B164" s="2">
@@ -6409,7 +6409,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A165" s="51" t="s">
+      <c r="A165" s="45" t="s">
         <v>193</v>
       </c>
       <c r="B165" s="2">
@@ -6422,7 +6422,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A166" s="51" t="s">
+      <c r="A166" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B166" s="2">
@@ -6435,7 +6435,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A167" s="51" t="s">
+      <c r="A167" s="45" t="s">
         <v>161</v>
       </c>
       <c r="B167" s="2">
@@ -6448,7 +6448,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A168" s="51" t="s">
+      <c r="A168" s="45" t="s">
         <v>58</v>
       </c>
       <c r="B168" s="2">
@@ -6461,7 +6461,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A169" s="51" t="s">
+      <c r="A169" s="45" t="s">
         <v>91</v>
       </c>
       <c r="B169" s="2">
@@ -6474,7 +6474,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170" s="51" t="s">
+      <c r="A170" s="45" t="s">
         <v>55</v>
       </c>
       <c r="B170" s="2">
@@ -6487,7 +6487,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" s="51" t="s">
+      <c r="A171" s="45" t="s">
         <v>83</v>
       </c>
       <c r="B171" s="2">
@@ -6500,7 +6500,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172" s="51" t="s">
+      <c r="A172" s="45" t="s">
         <v>94</v>
       </c>
       <c r="B172" s="2">
@@ -6513,7 +6513,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173" s="51" t="s">
+      <c r="A173" s="45" t="s">
         <v>169</v>
       </c>
       <c r="B173" s="2">
@@ -6792,86 +6792,86 @@
       <c r="A1" s="32">
         <v>2001</v>
       </c>
-      <c r="B1" s="45">
+      <c r="B1" s="48">
         <v>2002</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48">
         <v>2003</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48">
         <v>2004</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45">
+      <c r="G1" s="48"/>
+      <c r="H1" s="48">
         <v>2005</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45">
+      <c r="I1" s="48"/>
+      <c r="J1" s="48">
         <v>2006</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45">
+      <c r="K1" s="48"/>
+      <c r="L1" s="48">
         <v>2007</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45">
+      <c r="M1" s="48"/>
+      <c r="N1" s="48">
         <v>2008</v>
       </c>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45">
+      <c r="O1" s="48"/>
+      <c r="P1" s="48">
         <v>2009</v>
       </c>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="47">
+      <c r="Q1" s="48"/>
+      <c r="R1" s="49">
         <v>2010</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="T1" s="46">
+      <c r="S1" s="50"/>
+      <c r="T1" s="47">
         <v>2011</v>
       </c>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46">
+      <c r="U1" s="47"/>
+      <c r="V1" s="47">
         <v>2012</v>
       </c>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46">
+      <c r="W1" s="47"/>
+      <c r="X1" s="47">
         <v>2013</v>
       </c>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46">
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47">
         <v>2014</v>
       </c>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46">
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47">
         <v>2015</v>
       </c>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46">
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47">
         <v>2016</v>
       </c>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46">
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47">
         <v>2017</v>
       </c>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46">
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47">
         <v>2018</v>
       </c>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46">
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47">
         <v>2019</v>
       </c>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46">
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47">
         <v>2021</v>
       </c>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46">
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47">
         <v>2022</v>
       </c>
-      <c r="AO1" s="46"/>
+      <c r="AO1" s="47"/>
     </row>
     <row r="2" spans="1:41" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
@@ -11339,6 +11339,18 @@
     <sortCondition ref="N2:N37"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
@@ -11347,18 +11359,6 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11381,13 +11381,13 @@
       <c r="A1" s="40" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">

</xml_diff>

<commit_message>
Team retention name change
</commit_message>
<xml_diff>
--- a/Docs/Data/Team Retention.xlsx
+++ b/Docs/Data/Team Retention.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vws1\Documents\Personal\Soccer\GKSSA-Stats-Calculator\Docs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537B059B-7E6C-4944-9944-62D822C7D55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E176B446-E12C-49E7-8055-13EA6C6CC4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{7844BBDF-6516-4F3E-ACF8-72B0D7E6BADF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{7844BBDF-6516-4F3E-ACF8-72B0D7E6BADF}"/>
   </bookViews>
   <sheets>
     <sheet name="Retention" sheetId="2" r:id="rId1"/>
@@ -702,10 +702,10 @@
     <t>5th Percentile</t>
   </si>
   <si>
-    <t>Original Team Name</t>
-  </si>
-  <si>
     <t>Alternate Names</t>
+  </si>
+  <si>
+    <t>Original Name</t>
   </si>
 </sst>
 </file>
@@ -1142,10 +1142,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4027,7 +4027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB03638-F2B9-49CE-B1BB-2BDDB09491D5}">
   <dimension ref="A1:J357"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F163" sqref="F163"/>
     </sheetView>
@@ -6792,86 +6792,86 @@
       <c r="A1" s="32">
         <v>2001</v>
       </c>
-      <c r="B1" s="48">
+      <c r="B1" s="47">
         <v>2002</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47">
         <v>2003</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48">
+      <c r="E1" s="47"/>
+      <c r="F1" s="47">
         <v>2004</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48">
+      <c r="G1" s="47"/>
+      <c r="H1" s="47">
         <v>2005</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48">
+      <c r="I1" s="47"/>
+      <c r="J1" s="47">
         <v>2006</v>
       </c>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48">
+      <c r="K1" s="47"/>
+      <c r="L1" s="47">
         <v>2007</v>
       </c>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48">
+      <c r="M1" s="47"/>
+      <c r="N1" s="47">
         <v>2008</v>
       </c>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48">
+      <c r="O1" s="47"/>
+      <c r="P1" s="47">
         <v>2009</v>
       </c>
-      <c r="Q1" s="48"/>
+      <c r="Q1" s="47"/>
       <c r="R1" s="49">
         <v>2010</v>
       </c>
       <c r="S1" s="50"/>
-      <c r="T1" s="47">
+      <c r="T1" s="48">
         <v>2011</v>
       </c>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47">
+      <c r="U1" s="48"/>
+      <c r="V1" s="48">
         <v>2012</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47">
+      <c r="W1" s="48"/>
+      <c r="X1" s="48">
         <v>2013</v>
       </c>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47">
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48">
         <v>2014</v>
       </c>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47">
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48">
         <v>2015</v>
       </c>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47">
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48">
         <v>2016</v>
       </c>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47">
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48">
         <v>2017</v>
       </c>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="47">
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="48">
         <v>2018</v>
       </c>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47">
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="48">
         <v>2019</v>
       </c>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="47">
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="48">
         <v>2021</v>
       </c>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="47">
+      <c r="AM1" s="48"/>
+      <c r="AN1" s="48">
         <v>2022</v>
       </c>
-      <c r="AO1" s="47"/>
+      <c r="AO1" s="48"/>
     </row>
     <row r="2" spans="1:41" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
@@ -11339,18 +11339,6 @@
     <sortCondition ref="N2:N37"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
@@ -11359,6 +11347,18 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11368,7 +11368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF1E22A-C9B0-4903-9FFB-118C472359E0}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -11379,10 +11379,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="40" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>221</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>222</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>

</xml_diff>